<commit_message>
Fix colors and errors on the excel sheet
</commit_message>
<xml_diff>
--- a/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
+++ b/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460ED58F-C052-8844-82ED-7F02849699BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C7317E-59BF-0440-9A86-E157EDBFB29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
   <si>
     <t>library_urn</t>
   </si>
@@ -138,9 +138,6 @@
     <t>library_description[fr]</t>
   </si>
   <si>
-    <t>risk_matrix_name[fr]</t>
-  </si>
-  <si>
     <t>risk_matrix_description[fr]</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>4x4 risk matrix from EBIOS-RM</t>
   </si>
   <si>
-    <t>urn:intuitem:risk:matrix:4x4-ebios-rm</t>
-  </si>
-  <si>
     <t>Matrice 4x4 EBIOS-RM</t>
   </si>
   <si>
@@ -255,18 +249,12 @@
     <t>La source de risque va certainement atteindre son objectif visé selon l’un des modes opératoires envisagés OU un tel scénario s’est déjà produit au sein de l’organisation (historique d’incidents).</t>
   </si>
   <si>
-    <t>The source of risk will certainly achieve its intended purpose in one of the envisaged modes of operation OR such a scenario has already occurred within the organization (incident history).</t>
-  </si>
-  <si>
     <t>The source of risk is unlikely to achieve its intended objective under any of the proposed procedures. The likelihood of the scenario is weak.</t>
   </si>
   <si>
     <t xml:space="preserve"> The source of risk is likely to achieve its intended objective according to one of the operating procedures envisaged. The likelihood of the scenario is significant. </t>
   </si>
   <si>
-    <t>The source of risk is likely to achieve its intended purpose in one of the ways in which it is considered. The likelihood of the scenario is high.</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -276,9 +264,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Acceptable as it stands. No action required.</t>
-  </si>
-  <si>
     <t>Acceptable en l'état</t>
   </si>
   <si>
@@ -297,12 +282,6 @@
     <t>Inacceptable. Des mesures de réduction du risque doivent impérativement être prises à court terme. Dans le cas contraire, tout ou partie de l’activité sera refusée.</t>
   </si>
   <si>
-    <t>Tolerable under control. Monitoring in terms of risk management must be carried out and actions must be put in place as part of continuous improvement over the medium and long term.</t>
-  </si>
-  <si>
-    <t>Unacceptable. It is imperative that risk reduction measures be taken in the short term. Otherwise, all or part of the activity will be refused.</t>
-  </si>
-  <si>
     <t>G1</t>
   </si>
   <si>
@@ -313,6 +292,30 @@
   </si>
   <si>
     <t>G4</t>
+  </si>
+  <si>
+    <t>The risk source will certainly achieve its intended objective through one of the anticipated methods of operation OR such a scenario has already occurred within the organization (incident history).</t>
+  </si>
+  <si>
+    <t>The risk source is very likely to achieve its intended objective through one of the anticipated methods of operation. The likelihood of the scenario is high.</t>
+  </si>
+  <si>
+    <t>Acceptable as is.</t>
+  </si>
+  <si>
+    <t>Tolerable under control. Risk management monitoring must be conducted, and actions should be implemented as part of continuous improvement in the medium and long term.</t>
+  </si>
+  <si>
+    <t>Unacceptable. Risk reduction measures must be implemented urgently in the short term. Otherwise, all or part of the activity will be denied.</t>
+  </si>
+  <si>
+    <t>based on the official guide of the EBIOS RM approach</t>
+  </si>
+  <si>
+    <t>Basée sur le guide officiel de la méthode EBIOS RM</t>
+  </si>
+  <si>
+    <t>urn:intuitem:risk:matrix:risk-matrix-4x4-ebios-rm</t>
   </si>
 </sst>
 </file>
@@ -335,7 +338,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,25 +347,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA600"/>
+        <fgColor rgb="FF42C7C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFC586"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFEE7B86"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCE02"/>
+        <fgColor rgb="FFE6686D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5C481"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF59BBB2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBF082"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4AA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCCC77"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEE6BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAF7E9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -426,12 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -442,25 +481,46 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -471,13 +531,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFFCE02"/>
-      <color rgb="FFFFA600"/>
-      <color rgb="FFD3FF4E"/>
-      <color rgb="FFFF1A00"/>
-      <color rgb="FF02A45A"/>
-      <color rgb="FFEAFF03"/>
-      <color rgb="FFF4FF66"/>
+      <color rgb="FFFAF7E9"/>
+      <color rgb="FFEEE6BC"/>
+      <color rgb="FFDCCC77"/>
+      <color rgb="FFC4AA00"/>
+      <color rgb="FF42C7C4"/>
+      <color rgb="FFFBF082"/>
+      <color rgb="FFFFC586"/>
+      <color rgb="FFEE7B86"/>
+      <color rgb="FF59BBB2"/>
+      <color rgb="FFF5C481"/>
     </mruColors>
   </colors>
   <extLst>
@@ -810,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="177" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -850,7 +913,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -858,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -866,7 +929,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -874,7 +937,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -898,7 +961,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,7 +969,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -914,7 +977,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -922,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -941,7 +1004,7 @@
         <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -949,23 +1012,23 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -978,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="140" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,10 +1051,10 @@
     <col min="2" max="2" width="4.33203125" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="77.6640625" style="8" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="2"/>
     <col min="11" max="11" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="76" style="11" customWidth="1"/>
+    <col min="12" max="12" width="76" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1010,7 +1073,7 @@
       <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1026,10 +1089,10 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -1039,33 +1102,33 @@
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="8" t="s">
-        <v>60</v>
+      <c r="C2" s="17"/>
+      <c r="D2" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" s="14">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
+        <v>2</v>
+      </c>
+      <c r="J2" s="13">
+        <v>2</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1</v>
-      </c>
-      <c r="I2" s="15">
-        <v>2</v>
-      </c>
-      <c r="J2" s="15">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1075,33 +1138,33 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8" t="s">
-        <v>59</v>
+      <c r="C3" s="18"/>
+      <c r="D3" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="15">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="13">
+        <v>2</v>
+      </c>
+      <c r="J3" s="13">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="9">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15">
-        <v>2</v>
-      </c>
-      <c r="J3" s="15">
-        <v>2</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1111,33 +1174,33 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="8" t="s">
-        <v>57</v>
+      <c r="C4" s="19"/>
+      <c r="D4" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="9">
+        <v>61</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="15">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="15">
         <v>0</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="14">
         <v>1</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="13">
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1147,33 +1210,33 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="8" t="s">
-        <v>58</v>
+      <c r="C5" s="20"/>
+      <c r="D5" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="9">
+        <v>60</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="15">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="15">
         <v>0</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="14">
         <v>1</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="14">
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1183,21 +1246,21 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8" t="s">
-        <v>88</v>
+      <c r="C6" s="10"/>
+      <c r="D6" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>53</v>
+        <v>42</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1207,21 +1270,21 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="8" t="s">
-        <v>89</v>
+      <c r="C7" s="16"/>
+      <c r="D7" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>54</v>
+        <v>43</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1231,21 +1294,21 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="8" t="s">
-        <v>90</v>
+      <c r="C8" s="11"/>
+      <c r="D8" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1256,20 +1319,20 @@
         <v>3</v>
       </c>
       <c r="C9" s="12"/>
-      <c r="D9" s="8" t="s">
-        <v>91</v>
+      <c r="D9" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>54</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1279,21 +1342,21 @@
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="L10" s="10" t="s">
-        <v>80</v>
+      <c r="E10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -1303,21 +1366,21 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L11" s="10" t="s">
-        <v>81</v>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1327,25 +1390,25 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>85</v>
+      <c r="E12" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F13" s="10"/>
+      <c r="F13" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix the Ebios RM matrix
</commit_message>
<xml_diff>
--- a/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
+++ b/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C7317E-59BF-0440-9A86-E157EDBFB29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0B23ED-24F4-014E-90F8-93E13937D7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="3860" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
   <si>
     <t>library_urn</t>
   </si>
@@ -162,24 +162,6 @@
     <t>Matrice 4x4 EBIOS-RM</t>
   </si>
   <si>
-    <t>G1 - Mineur</t>
-  </si>
-  <si>
-    <t>G1 - Minor</t>
-  </si>
-  <si>
-    <t>G2 - Significant</t>
-  </si>
-  <si>
-    <t>G2 - Significatif</t>
-  </si>
-  <si>
-    <t>G3 - Important</t>
-  </si>
-  <si>
-    <t>G4 - Critique</t>
-  </si>
-  <si>
     <t>Aucun impact opérationnel ni sur les performances de l’activité ni sur la sécurité des personnes et des biens.</t>
   </si>
   <si>
@@ -216,33 +198,12 @@
     <t>V4</t>
   </si>
   <si>
-    <t>V1 - Peu vraisemblable</t>
-  </si>
-  <si>
-    <t>V1 - Implausible</t>
-  </si>
-  <si>
-    <t>V2 - Plausible</t>
-  </si>
-  <si>
-    <t>V2 - Vraisemblable</t>
-  </si>
-  <si>
     <t>La source de risque a peu de chances d’atteindre son objectif visé selon l’un des modes opératoires envisagés. La vraisemblance du scénario est faible.</t>
   </si>
   <si>
     <t>La source de risque est susceptible d’atteindre son objectif visé selon l’un des modes opératoires envisagés. La vraisemblance du scénario est significative.</t>
   </si>
   <si>
-    <t>V3 - Très vraisemblable</t>
-  </si>
-  <si>
-    <t>V3 - Very likely</t>
-  </si>
-  <si>
-    <t>V4 - Certain</t>
-  </si>
-  <si>
     <t>La source de risque va probablement atteindre son objectif visé selon l’un des modes opératoires envisagés. La vraisemblance du scénario est élevée.</t>
   </si>
   <si>
@@ -316,6 +277,48 @@
   </si>
   <si>
     <t>urn:intuitem:risk:matrix:risk-matrix-4x4-ebios-rm</t>
+  </si>
+  <si>
+    <t>Certain</t>
+  </si>
+  <si>
+    <t>Très vraisemblable</t>
+  </si>
+  <si>
+    <t>Vraisemblable</t>
+  </si>
+  <si>
+    <t>Peu vraisemblable</t>
+  </si>
+  <si>
+    <t>Mineur</t>
+  </si>
+  <si>
+    <t>Significatif</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>Critique</t>
+  </si>
+  <si>
+    <t>Very likely</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Significant</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Likely</t>
+  </si>
+  <si>
+    <t>Unlikely</t>
   </si>
 </sst>
 </file>
@@ -873,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="177" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,7 +932,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -961,7 +964,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -985,7 +988,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1012,12 +1015,12 @@
         <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>40</v>
@@ -1028,7 +1031,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1041,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1104,13 +1107,13 @@
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G2" s="14">
         <v>1</v>
@@ -1125,10 +1128,10 @@
         <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1140,13 +1143,13 @@
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="G3" s="15">
         <v>0</v>
@@ -1161,10 +1164,10 @@
         <v>2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1176,13 +1179,13 @@
       </c>
       <c r="C4" s="19"/>
       <c r="D4" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="G4" s="15">
         <v>0</v>
@@ -1197,10 +1200,10 @@
         <v>2</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1212,13 +1215,13 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G5" s="15">
         <v>0</v>
@@ -1233,10 +1236,10 @@
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1248,19 +1251,19 @@
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1272,19 +1275,19 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="6" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1296,19 +1299,19 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="6" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1320,19 +1323,19 @@
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="6" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -1347,16 +1350,16 @@
         <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="51" x14ac:dyDescent="0.2">
@@ -1371,16 +1374,16 @@
         <v>29</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="34" x14ac:dyDescent="0.2">
@@ -1395,16 +1398,16 @@
         <v>30</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix(lib): EBIOS-RM matrix (#1935)
</commit_message>
<xml_diff>
--- a/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
+++ b/tools/matrix/risk-matrix-4x4-ebios-rm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE16766-2DDC-2A45-B2F6-C7A88AC9BDC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA767CD4-4D86-FF44-A17A-FD349432CBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20580" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -880,7 +880,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1047,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,8 +1121,8 @@
       <c r="G2" s="14">
         <v>1</v>
       </c>
-      <c r="H2" s="14">
-        <v>1</v>
+      <c r="H2" s="13">
+        <v>2</v>
       </c>
       <c r="I2" s="13">
         <v>2</v>
@@ -1154,8 +1154,8 @@
       <c r="F3" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="15">
-        <v>0</v>
+      <c r="G3" s="14">
+        <v>1</v>
       </c>
       <c r="H3" s="14">
         <v>1</v>
@@ -1199,8 +1199,8 @@
       <c r="I4" s="14">
         <v>1</v>
       </c>
-      <c r="J4" s="13">
-        <v>2</v>
+      <c r="J4" s="14">
+        <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>82</v>
@@ -1232,8 +1232,8 @@
       <c r="H5" s="15">
         <v>0</v>
       </c>
-      <c r="I5" s="14">
-        <v>1</v>
+      <c r="I5" s="15">
+        <v>0</v>
       </c>
       <c r="J5" s="14">
         <v>1</v>

</xml_diff>